<commit_message>
Update: Need to use long long int for not overflow the result
</commit_message>
<xml_diff>
--- a/Codeforces/ProlemsSolved_Record.xlsx
+++ b/Codeforces/ProlemsSolved_Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project C++\Data-Structures-and-Algorithms\Codeforces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BD31DD-DDFE-40A6-B5DB-9ABB17566C93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E09A17E-51ED-4EFD-BE3C-809D8D7A6808}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{99512D60-B3F3-4EAE-B85D-FB965F1F4D51}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>http://codeforces.com/problemset/problem/1/A</t>
   </si>
   <si>
-    <t>Answer = ceil(m/a) * ceil(n/a), where ceil(x) is the least integer which is above or equal to x. Using integers only, it is usually written as ((m+a-1)/a)*((n+a-1)/a). *Note: Using double for the result.</t>
+    <t>Answer = ceil(m/a) * ceil(n/a), where ceil(x) is the least integer which is above or equal to x. Using integers only, it is usually written as ((m+a-1)/a)*((n+a-1)/a). *Note: Using long long int for the result.</t>
   </si>
 </sst>
 </file>
@@ -309,22 +309,22 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -336,7 +336,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -348,20 +354,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -685,7 +685,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="H3" sqref="H3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,53 +695,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="1" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="17">
+      <c r="A3" s="1">
         <v>43225</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="7" t="s">
         <v>5</v>
       </c>
@@ -751,13 +751,13 @@
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="7"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -765,13 +765,13 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -779,13 +779,13 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="7"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -793,13 +793,13 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="7"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -807,13 +807,13 @@
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -821,13 +821,13 @@
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -835,13 +835,13 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -849,13 +849,13 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="7"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -863,13 +863,13 @@
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="7"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -877,13 +877,13 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
       <c r="H13" s="7"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -891,13 +891,13 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="7"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -905,13 +905,13 @@
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="7"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -919,13 +919,13 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="7"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -933,13 +933,13 @@
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
       <c r="H17" s="7"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -947,13 +947,13 @@
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="7"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -961,13 +961,13 @@
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="7"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -975,13 +975,13 @@
       <c r="L19" s="9"/>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
       <c r="H20" s="7"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -989,13 +989,13 @@
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
       <c r="H21" s="7"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -1003,13 +1003,13 @@
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15"/>
       <c r="H22" s="7"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1017,13 +1017,13 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
       <c r="H23" s="7"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -1031,13 +1031,13 @@
       <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15"/>
       <c r="H24" s="7"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -1045,13 +1045,13 @@
       <c r="L24" s="9"/>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="17"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="7"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -1059,13 +1059,13 @@
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="15"/>
       <c r="H26" s="7"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -1073,13 +1073,13 @@
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
       <c r="H27" s="7"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -1087,13 +1087,13 @@
       <c r="L27" s="9"/>
     </row>
     <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -1101,13 +1101,13 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="17"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="15"/>
       <c r="H29" s="7"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
@@ -1115,13 +1115,13 @@
       <c r="L29" s="9"/>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="17"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="13"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
       <c r="H30" s="7"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
@@ -1129,13 +1129,13 @@
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="17"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="13"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15"/>
       <c r="H31" s="7"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
@@ -1143,13 +1143,13 @@
       <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="17"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="13"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="15"/>
       <c r="H32" s="7"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
@@ -1157,13 +1157,13 @@
       <c r="L32" s="9"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="17"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="13"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
       <c r="H33" s="7"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
@@ -1171,13 +1171,13 @@
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="17"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="13"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15"/>
       <c r="H34" s="7"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -1185,13 +1185,13 @@
       <c r="L34" s="9"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="17"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="13"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15"/>
       <c r="H35" s="7"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
@@ -1199,13 +1199,13 @@
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="17"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="13"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="15"/>
       <c r="H36" s="7"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
@@ -1213,13 +1213,13 @@
       <c r="L36" s="9"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="17"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="13"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="7"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
@@ -1227,13 +1227,13 @@
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="17"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="13"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="15"/>
       <c r="H38" s="7"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
@@ -1241,13 +1241,13 @@
       <c r="L38" s="9"/>
     </row>
     <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="17"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="13"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="15"/>
       <c r="H39" s="7"/>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
@@ -1255,13 +1255,13 @@
       <c r="L39" s="9"/>
     </row>
     <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="17"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="15"/>
       <c r="H40" s="7"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
@@ -1269,13 +1269,13 @@
       <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="13"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="15"/>
       <c r="H41" s="7"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
@@ -1283,13 +1283,13 @@
       <c r="L41" s="9"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="17"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="13"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="15"/>
       <c r="H42" s="7"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -1297,13 +1297,13 @@
       <c r="L42" s="9"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="17"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
       <c r="H43" s="7"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
@@ -1311,13 +1311,13 @@
       <c r="L43" s="9"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="17"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="13"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="15"/>
       <c r="H44" s="7"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
@@ -1325,13 +1325,13 @@
       <c r="L44" s="9"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="17"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="13"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="15"/>
       <c r="H45" s="7"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
@@ -1339,13 +1339,13 @@
       <c r="L45" s="9"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="17"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="13"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="15"/>
       <c r="H46" s="7"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
@@ -1353,13 +1353,13 @@
       <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="17"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="13"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
       <c r="H47" s="7"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
@@ -1367,13 +1367,13 @@
       <c r="L47" s="9"/>
     </row>
     <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="17"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="13"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="15"/>
       <c r="H48" s="7"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
@@ -1381,13 +1381,13 @@
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="17"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="13"/>
+      <c r="A49" s="1"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="15"/>
       <c r="H49" s="7"/>
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
@@ -1395,13 +1395,13 @@
       <c r="L49" s="9"/>
     </row>
     <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="17"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="13"/>
+      <c r="A50" s="1"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="15"/>
       <c r="H50" s="7"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
@@ -1409,13 +1409,13 @@
       <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="17"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="13"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="15"/>
       <c r="H51" s="7"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
@@ -1423,13 +1423,13 @@
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="17"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="13"/>
+      <c r="A52" s="1"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="15"/>
       <c r="H52" s="7"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
@@ -1437,13 +1437,13 @@
       <c r="L52" s="9"/>
     </row>
     <row r="53" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="17"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="13"/>
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="15"/>
       <c r="H53" s="7"/>
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
@@ -1451,13 +1451,13 @@
       <c r="L53" s="9"/>
     </row>
     <row r="54" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="17"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="13"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="15"/>
       <c r="H54" s="7"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
@@ -1465,13 +1465,13 @@
       <c r="L54" s="9"/>
     </row>
     <row r="55" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="17"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="13"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="15"/>
       <c r="H55" s="7"/>
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
@@ -1479,13 +1479,13 @@
       <c r="L55" s="9"/>
     </row>
     <row r="56" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="17"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="13"/>
+      <c r="A56" s="1"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="15"/>
       <c r="H56" s="7"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
@@ -1493,13 +1493,13 @@
       <c r="L56" s="9"/>
     </row>
     <row r="57" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="17"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="13"/>
+      <c r="A57" s="1"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="15"/>
       <c r="H57" s="7"/>
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
@@ -1507,13 +1507,13 @@
       <c r="L57" s="9"/>
     </row>
     <row r="58" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="17"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="13"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="15"/>
       <c r="H58" s="7"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
@@ -1521,13 +1521,13 @@
       <c r="L58" s="9"/>
     </row>
     <row r="59" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="17"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="13"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="15"/>
       <c r="H59" s="7"/>
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
@@ -1536,29 +1536,128 @@
     </row>
   </sheetData>
   <mergeCells count="175">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="H55:L55"/>
+    <mergeCell ref="H56:L56"/>
+    <mergeCell ref="H57:L57"/>
+    <mergeCell ref="H58:L58"/>
+    <mergeCell ref="H59:L59"/>
+    <mergeCell ref="H49:L49"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="H51:L51"/>
+    <mergeCell ref="H52:L52"/>
+    <mergeCell ref="H53:L53"/>
+    <mergeCell ref="H54:L54"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="H45:L45"/>
+    <mergeCell ref="H46:L46"/>
+    <mergeCell ref="H47:L47"/>
+    <mergeCell ref="H48:L48"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="H24:L24"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="C2:G2"/>
@@ -1583,134 +1682,35 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="H6:L6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="H5:L5"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="H22:L22"/>
-    <mergeCell ref="H23:L23"/>
-    <mergeCell ref="H24:L24"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="H33:L33"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="H25:L25"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="H45:L45"/>
-    <mergeCell ref="H46:L46"/>
-    <mergeCell ref="H47:L47"/>
-    <mergeCell ref="H48:L48"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="H55:L55"/>
-    <mergeCell ref="H56:L56"/>
-    <mergeCell ref="H57:L57"/>
-    <mergeCell ref="H58:L58"/>
-    <mergeCell ref="H59:L59"/>
-    <mergeCell ref="H49:L49"/>
-    <mergeCell ref="H50:L50"/>
-    <mergeCell ref="H51:L51"/>
-    <mergeCell ref="H52:L52"/>
-    <mergeCell ref="H53:L53"/>
-    <mergeCell ref="H54:L54"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{BE45FD94-71F5-4056-B6E5-4434C4B202D9}"/>

</xml_diff>